<commit_message>
Nebraska water rights update.
Nebraska water rights update.
</commit_message>
<xml_diff>
--- a/Nebraska/WaterAllocation/NE_Allocation Schema Mapping to WaDE_QA.xlsx
+++ b/Nebraska/WaterAllocation/NE_Allocation Schema Mapping to WaDE_QA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjame\Documents\WSWC Documents\MappingStatesDataToWaDE2.0\Nebraska\WaterAllocation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70A6BD7B-9EEB-4C41-B624-2013330BF726}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA2DDA81-5B7D-4A3D-80FA-44A9E893380A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="1692" windowWidth="23256" windowHeight="12576" tabRatio="714" firstSheet="1" activeTab="6" xr2:uid="{10FC1BAB-5472-410C-A2F0-85DCDF5389F8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="714" activeTab="6" xr2:uid="{10FC1BAB-5472-410C-A2F0-85DCDF5389F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping Notes" sheetId="10" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1122" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1129" uniqueCount="398">
   <si>
     <t>Name</t>
   </si>
@@ -758,9 +758,6 @@
   </si>
   <si>
     <t>State:</t>
-  </si>
-  <si>
-    <t>Organizaitons:</t>
   </si>
   <si>
     <t>Data Links:</t>
@@ -1159,9 +1156,6 @@
     <t>Questions</t>
   </si>
   <si>
-    <t>Do they use water year or calender year?</t>
-  </si>
-  <si>
     <t>01/01</t>
   </si>
   <si>
@@ -1171,9 +1165,6 @@
     <t>This field contains the Type of Application or Water Right of this database entry. examples: Underground Water Claim, Federal Reserved Water Right</t>
   </si>
   <si>
-    <t>Do they have something equilvalent to an allowcation type field?</t>
-  </si>
-  <si>
     <t>RightUse</t>
   </si>
   <si>
@@ -1204,12 +1195,6 @@
     <t>Provide Nebraskas citizens and leaders with the data and analyses they need to make wise resource decisions for the benefit of all Nebraskans both now and in the future.</t>
   </si>
   <si>
-    <t>Use above API to retreie surface water data.  Will merge with POD shapefile data vie RightID.</t>
-  </si>
-  <si>
-    <t>Shapefile data with location info from email corespondance.</t>
-  </si>
-  <si>
     <t>PODorPOUSite</t>
   </si>
   <si>
@@ -1238,6 +1223,30 @@
   </si>
   <si>
     <t>AllocationFlow_AF</t>
+  </si>
+  <si>
+    <t>Do they use water year or calendar year?</t>
+  </si>
+  <si>
+    <t>Do they have something equivalent to an allocation type field?</t>
+  </si>
+  <si>
+    <t>Organizations:</t>
+  </si>
+  <si>
+    <t>Shapefile data with location info from email correspondence.</t>
+  </si>
+  <si>
+    <t>Use above API to retrieve surface water data.  Will merge with POD shapefile data vie RightID.</t>
+  </si>
+  <si>
+    <t>OwnerClassificationCV</t>
+  </si>
+  <si>
+    <t>Army (USA)</t>
+  </si>
+  <si>
+    <t>WSWC defined owner tag.</t>
   </si>
 </sst>
 </file>
@@ -2029,7 +2038,7 @@
     <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2326,6 +2335,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -2686,7 +2698,7 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2700,15 +2712,15 @@
         <v>238</v>
       </c>
       <c r="B1" s="75" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="75" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="71" t="s">
-        <v>239</v>
+        <v>392</v>
       </c>
       <c r="B2" s="75" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="75" customFormat="1" x14ac:dyDescent="0.3">
@@ -2716,16 +2728,16 @@
     </row>
     <row r="4" spans="1:2" s="75" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="71" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B4" s="94" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="5" spans="1:2" s="75" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="71"/>
       <c r="B5" s="93" t="s">
-        <v>384</v>
+        <v>393</v>
       </c>
     </row>
     <row r="6" spans="1:2" s="75" customFormat="1" x14ac:dyDescent="0.3">
@@ -2737,27 +2749,27 @@
     </row>
     <row r="8" spans="1:2" s="75" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="71" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B8" s="75" t="s">
-        <v>383</v>
+        <v>394</v>
       </c>
     </row>
     <row r="9" spans="1:2" s="75" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="71"/>
       <c r="B9" s="75" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="10" spans="1:2" s="75" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="71"/>
       <c r="B10" s="75" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B11" s="75" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -2768,20 +2780,20 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="71" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B15" t="s">
-        <v>368</v>
+        <v>390</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>372</v>
+        <v>391</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>
@@ -2901,7 +2913,7 @@
         <v>38</v>
       </c>
       <c r="E4" s="58" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="F4" s="45"/>
       <c r="G4" s="46"/>
@@ -2909,7 +2921,7 @@
         <v>38</v>
       </c>
       <c r="I4" s="17" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="J4" s="62" t="s">
         <v>190</v>
@@ -3041,7 +3053,7 @@
         <v>38</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="F9" s="20"/>
       <c r="G9" s="21"/>
@@ -3067,7 +3079,7 @@
         <v>38</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="F10" s="20"/>
       <c r="G10" s="21"/>
@@ -3254,7 +3266,7 @@
         <v>38</v>
       </c>
       <c r="E4" s="85" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="F4" s="45" t="s">
         <v>38</v>
@@ -3677,7 +3689,7 @@
         <v>38</v>
       </c>
       <c r="E4" s="43" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F4" s="45" t="s">
         <v>38</v>
@@ -3709,7 +3721,7 @@
         <v>38</v>
       </c>
       <c r="E5" s="92" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F5" s="20" t="s">
         <v>38</v>
@@ -3741,7 +3753,7 @@
         <v>38</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F6" s="20" t="s">
         <v>38</v>
@@ -3773,7 +3785,7 @@
         <v>38</v>
       </c>
       <c r="E7" s="91" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F7" s="20" t="s">
         <v>38</v>
@@ -3805,7 +3817,7 @@
         <v>38</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="F8" s="20" t="s">
         <v>38</v>
@@ -3837,7 +3849,7 @@
         <v>38</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F9" s="20" t="s">
         <v>38</v>
@@ -3869,7 +3881,7 @@
         <v>38</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="F10" s="20" t="s">
         <v>38</v>
@@ -3901,7 +3913,7 @@
         <v>38</v>
       </c>
       <c r="E11" s="91" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F11" s="20" t="s">
         <v>38</v>
@@ -3933,7 +3945,7 @@
         <v>38</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F12" s="20" t="s">
         <v>38</v>
@@ -4096,7 +4108,7 @@
         <v>38</v>
       </c>
       <c r="E4" s="81" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F4" s="82" t="s">
         <v>38</v>
@@ -4222,7 +4234,7 @@
         <v>38</v>
       </c>
       <c r="G8" s="84" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="H8" s="23"/>
       <c r="I8" s="17" t="s">
@@ -4413,7 +4425,7 @@
         <v>38</v>
       </c>
       <c r="E4" s="81" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F4" s="45" t="s">
         <v>38</v>
@@ -4473,7 +4485,7 @@
         <v>20</v>
       </c>
       <c r="E6" s="22" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F6" s="25" t="s">
         <v>38</v>
@@ -4509,7 +4521,7 @@
         <v>38</v>
       </c>
       <c r="G7" s="26" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="H7" s="19"/>
       <c r="I7" s="22" t="s">
@@ -4789,7 +4801,7 @@
     </row>
     <row r="17" spans="1:10" s="51" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>16</v>
@@ -4801,7 +4813,7 @@
         <v>38</v>
       </c>
       <c r="E17" s="64" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="F17" s="35" t="s">
         <v>38</v>
@@ -4811,7 +4823,7 @@
       </c>
       <c r="H17" s="95"/>
       <c r="I17" s="96" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="J17" s="95"/>
     </row>
@@ -4827,7 +4839,7 @@
         <v>38</v>
       </c>
       <c r="E18" s="22" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F18" s="25" t="s">
         <v>38</v>
@@ -4863,7 +4875,7 @@
         <v>38</v>
       </c>
       <c r="G19" s="26" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="H19" s="23"/>
       <c r="I19" s="18">
@@ -4947,7 +4959,7 @@
         <v>20</v>
       </c>
       <c r="E22" s="25" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F22" s="25" t="s">
         <v>38</v>
@@ -5004,10 +5016,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B91B1FF-D207-4871-B787-27544A9D3030}">
-  <dimension ref="A1:J46"/>
+  <dimension ref="A1:P47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="A43" sqref="A43:XFD43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5264,7 +5276,7 @@
         <v>38</v>
       </c>
       <c r="E9" s="89" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="F9" s="57" t="s">
         <v>38</v>
@@ -5296,7 +5308,7 @@
         <v>38</v>
       </c>
       <c r="E10" s="59" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F10" s="57" t="s">
         <v>38</v>
@@ -5328,7 +5340,7 @@
         <v>38</v>
       </c>
       <c r="E11" s="59" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="F11" s="57" t="s">
         <v>38</v>
@@ -5360,7 +5372,7 @@
         <v>38</v>
       </c>
       <c r="E12" s="90" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="F12" s="57" t="s">
         <v>38</v>
@@ -5392,7 +5404,7 @@
         <v>38</v>
       </c>
       <c r="E13" s="43" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F13" s="45" t="s">
         <v>38</v>
@@ -5668,7 +5680,7 @@
     </row>
     <row r="22" spans="1:10" s="51" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A22" s="97" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="B22" s="52" t="s">
         <v>69</v>
@@ -5680,11 +5692,11 @@
         <v>38</v>
       </c>
       <c r="E22" s="35" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="F22" s="64"/>
       <c r="G22" s="84" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="H22" s="98" t="s">
         <v>38</v>
@@ -5716,7 +5728,7 @@
         <v>38</v>
       </c>
       <c r="G23" s="21" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="H23" s="39" t="s">
         <v>38</v>
@@ -5748,7 +5760,7 @@
         <v>38</v>
       </c>
       <c r="G24" s="21" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="H24" s="39" t="s">
         <v>38</v>
@@ -5806,11 +5818,11 @@
         <v>20</v>
       </c>
       <c r="E26" s="25" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F26" s="35"/>
       <c r="G26" s="21" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="H26" s="39" t="s">
         <v>38</v>
@@ -5868,7 +5880,7 @@
         <v>38</v>
       </c>
       <c r="E28" s="72" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="F28" s="35"/>
       <c r="G28" s="21"/>
@@ -5896,7 +5908,7 @@
         <v>38</v>
       </c>
       <c r="E29" s="72" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="F29" s="35"/>
       <c r="G29" s="21"/>
@@ -5939,12 +5951,12 @@
         <v>133</v>
       </c>
       <c r="J30" s="62" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="31" spans="1:10" s="51" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A31" s="97" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="B31" s="52" t="s">
         <v>69</v>
@@ -5956,11 +5968,11 @@
         <v>38</v>
       </c>
       <c r="E31" s="35" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="F31" s="64"/>
       <c r="G31" s="84" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="H31" s="98" t="s">
         <v>38</v>
@@ -5986,11 +5998,11 @@
         <v>38</v>
       </c>
       <c r="E32" s="61" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="F32" s="35"/>
       <c r="G32" s="21" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H32" s="39" t="s">
         <v>38</v>
@@ -6002,7 +6014,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>101</v>
       </c>
@@ -6034,7 +6046,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>98</v>
       </c>
@@ -6066,7 +6078,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="35" spans="1:10" s="51" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:16" s="51" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>100</v>
       </c>
@@ -6098,7 +6110,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36" s="51" t="s">
         <v>154</v>
       </c>
@@ -6126,7 +6138,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>82</v>
       </c>
@@ -6158,12 +6170,12 @@
         <v>160</v>
       </c>
     </row>
-    <row r="38" spans="1:10" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:16" s="51" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="97" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="B38" s="52" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="C38" s="53" t="s">
         <v>18</v>
@@ -6184,7 +6196,7 @@
       <c r="I38" s="101"/>
       <c r="J38" s="102"/>
     </row>
-    <row r="39" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:16" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>90</v>
       </c>
@@ -6216,7 +6228,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>91</v>
       </c>
@@ -6246,7 +6258,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
         <v>99</v>
       </c>
@@ -6278,7 +6290,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>96</v>
       </c>
@@ -6310,50 +6322,50 @@
         <v>160</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:16" s="51" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
-        <v>89</v>
+        <v>395</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C43" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D43" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E43" s="25" t="s">
-        <v>159</v>
-      </c>
-      <c r="F43" s="35" t="s">
-        <v>38</v>
-      </c>
-      <c r="G43" s="48" t="s">
-        <v>38</v>
-      </c>
+      <c r="D43" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="103"/>
       <c r="H43" s="39" t="s">
         <v>38</v>
       </c>
       <c r="I43" s="66" t="s">
-        <v>38</v>
+        <v>396</v>
       </c>
       <c r="J43" s="62" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" s="51" customFormat="1" x14ac:dyDescent="0.3">
+        <v>397</v>
+      </c>
+      <c r="K43" s="5"/>
+      <c r="L43" s="5"/>
+      <c r="M43" s="5"/>
+      <c r="N43" s="5"/>
+      <c r="O43" s="5"/>
+      <c r="P43" s="5"/>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="C44" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="E44" s="25" t="s">
         <v>159</v>
@@ -6367,24 +6379,24 @@
       <c r="H44" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="I44" s="18" t="s">
-        <v>133</v>
-      </c>
-      <c r="J44" s="63" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A45" s="51" t="s">
-        <v>148</v>
-      </c>
-      <c r="B45" s="52" t="s">
-        <v>105</v>
-      </c>
-      <c r="C45" s="53" t="s">
+      <c r="I44" s="66" t="s">
+        <v>38</v>
+      </c>
+      <c r="J44" s="62" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" s="51" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C45" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D45" s="55" t="s">
+      <c r="D45" s="10" t="s">
         <v>20</v>
       </c>
       <c r="E45" s="25" t="s">
@@ -6399,25 +6411,25 @@
       <c r="H45" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="I45" s="64" t="s">
-        <v>132</v>
-      </c>
-      <c r="J45" s="62" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A46" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="B46" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C46" s="6" t="s">
+      <c r="I45" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="J45" s="63" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A46" s="51" t="s">
+        <v>148</v>
+      </c>
+      <c r="B46" s="52" t="s">
+        <v>105</v>
+      </c>
+      <c r="C46" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="D46" s="10" t="s">
-        <v>38</v>
+      <c r="D46" s="55" t="s">
+        <v>20</v>
       </c>
       <c r="E46" s="25" t="s">
         <v>159</v>
@@ -6431,16 +6443,48 @@
       <c r="H46" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="I46" s="18" t="s">
+      <c r="I46" s="64" t="s">
+        <v>132</v>
+      </c>
+      <c r="J46" s="62" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A47" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D47" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E47" s="25" t="s">
+        <v>159</v>
+      </c>
+      <c r="F47" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="G47" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="H47" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="I47" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="J46" s="62" t="s">
+      <c r="J47" s="62" t="s">
         <v>211</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A14:J46">
-    <sortCondition ref="A14:A46"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A14:J47">
+    <sortCondition ref="A14:A47"/>
   </sortState>
   <phoneticPr fontId="25" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6460,18 +6504,18 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="77" t="s">
+        <v>246</v>
+      </c>
+      <c r="B1" s="77" t="s">
         <v>247</v>
-      </c>
-      <c r="B1" s="77" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="78" t="s">
+        <v>248</v>
+      </c>
+      <c r="B2" s="78" t="s">
         <v>249</v>
-      </c>
-      <c r="B2" s="78" t="s">
-        <v>250</v>
       </c>
       <c r="H2" t="str">
         <f>""""&amp;TRIM(A2)&amp;""""&amp;" : "&amp;""""&amp;TRIM(B2)&amp;""""&amp;","</f>
@@ -6480,10 +6524,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="78" t="s">
+        <v>250</v>
+      </c>
+      <c r="B3" s="78" t="s">
         <v>251</v>
-      </c>
-      <c r="B3" s="78" t="s">
-        <v>252</v>
       </c>
       <c r="H3" t="str">
         <f t="shared" ref="H3:H39" si="0">""""&amp;TRIM(A3)&amp;""""&amp;" : "&amp;""""&amp;TRIM(B3)&amp;""""&amp;","</f>
@@ -6492,10 +6536,10 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="78" t="s">
+        <v>252</v>
+      </c>
+      <c r="B4" s="78" t="s">
         <v>253</v>
-      </c>
-      <c r="B4" s="78" t="s">
-        <v>254</v>
       </c>
       <c r="H4" t="str">
         <f t="shared" si="0"/>
@@ -6504,10 +6548,10 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="78" t="s">
+        <v>254</v>
+      </c>
+      <c r="B5" s="78" t="s">
         <v>255</v>
-      </c>
-      <c r="B5" s="78" t="s">
-        <v>256</v>
       </c>
       <c r="H5" t="str">
         <f t="shared" si="0"/>
@@ -6516,10 +6560,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="78" t="s">
+        <v>256</v>
+      </c>
+      <c r="B6" s="78" t="s">
         <v>257</v>
-      </c>
-      <c r="B6" s="78" t="s">
-        <v>258</v>
       </c>
       <c r="H6" t="str">
         <f t="shared" si="0"/>
@@ -6528,10 +6572,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="78" t="s">
+        <v>258</v>
+      </c>
+      <c r="B7" s="78" t="s">
         <v>259</v>
-      </c>
-      <c r="B7" s="78" t="s">
-        <v>260</v>
       </c>
       <c r="H7" t="str">
         <f t="shared" si="0"/>
@@ -6540,10 +6584,10 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="78" t="s">
+        <v>260</v>
+      </c>
+      <c r="B8" s="78" t="s">
         <v>261</v>
-      </c>
-      <c r="B8" s="78" t="s">
-        <v>262</v>
       </c>
       <c r="H8" t="str">
         <f t="shared" si="0"/>
@@ -6552,10 +6596,10 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="78" t="s">
+        <v>262</v>
+      </c>
+      <c r="B9" s="78" t="s">
         <v>263</v>
-      </c>
-      <c r="B9" s="78" t="s">
-        <v>264</v>
       </c>
       <c r="H9" t="str">
         <f t="shared" si="0"/>
@@ -6564,10 +6608,10 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="78" t="s">
+        <v>264</v>
+      </c>
+      <c r="B10" s="78" t="s">
         <v>265</v>
-      </c>
-      <c r="B10" s="78" t="s">
-        <v>266</v>
       </c>
       <c r="H10" t="str">
         <f t="shared" si="0"/>
@@ -6576,10 +6620,10 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="78" t="s">
+        <v>266</v>
+      </c>
+      <c r="B11" s="78" t="s">
         <v>267</v>
-      </c>
-      <c r="B11" s="78" t="s">
-        <v>268</v>
       </c>
       <c r="H11" t="str">
         <f t="shared" si="0"/>
@@ -6588,10 +6632,10 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="78" t="s">
+        <v>268</v>
+      </c>
+      <c r="B12" s="78" t="s">
         <v>269</v>
-      </c>
-      <c r="B12" s="78" t="s">
-        <v>270</v>
       </c>
       <c r="H12" t="str">
         <f t="shared" si="0"/>
@@ -6600,10 +6644,10 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="78" t="s">
+        <v>270</v>
+      </c>
+      <c r="B13" s="78" t="s">
         <v>271</v>
-      </c>
-      <c r="B13" s="78" t="s">
-        <v>272</v>
       </c>
       <c r="H13" t="str">
         <f t="shared" si="0"/>
@@ -6612,10 +6656,10 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="78" t="s">
+        <v>272</v>
+      </c>
+      <c r="B14" s="78" t="s">
         <v>273</v>
-      </c>
-      <c r="B14" s="78" t="s">
-        <v>274</v>
       </c>
       <c r="H14" t="str">
         <f t="shared" si="0"/>
@@ -6624,10 +6668,10 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="78" t="s">
+        <v>274</v>
+      </c>
+      <c r="B15" s="78" t="s">
         <v>275</v>
-      </c>
-      <c r="B15" s="78" t="s">
-        <v>276</v>
       </c>
       <c r="H15" t="str">
         <f t="shared" si="0"/>
@@ -6636,10 +6680,10 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="78" t="s">
+        <v>276</v>
+      </c>
+      <c r="B16" s="78" t="s">
         <v>277</v>
-      </c>
-      <c r="B16" s="78" t="s">
-        <v>278</v>
       </c>
       <c r="H16" t="str">
         <f t="shared" si="0"/>
@@ -6648,10 +6692,10 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="78" t="s">
+        <v>278</v>
+      </c>
+      <c r="B17" s="78" t="s">
         <v>279</v>
-      </c>
-      <c r="B17" s="78" t="s">
-        <v>280</v>
       </c>
       <c r="H17" t="str">
         <f t="shared" si="0"/>
@@ -6660,10 +6704,10 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="78" t="s">
+        <v>280</v>
+      </c>
+      <c r="B18" s="78" t="s">
         <v>281</v>
-      </c>
-      <c r="B18" s="78" t="s">
-        <v>282</v>
       </c>
       <c r="H18" t="str">
         <f t="shared" si="0"/>
@@ -6672,10 +6716,10 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="78" t="s">
+        <v>282</v>
+      </c>
+      <c r="B19" s="78" t="s">
         <v>283</v>
-      </c>
-      <c r="B19" s="78" t="s">
-        <v>284</v>
       </c>
       <c r="H19" t="str">
         <f t="shared" si="0"/>
@@ -6684,10 +6728,10 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="78" t="s">
+        <v>284</v>
+      </c>
+      <c r="B20" s="78" t="s">
         <v>285</v>
-      </c>
-      <c r="B20" s="78" t="s">
-        <v>286</v>
       </c>
       <c r="H20" t="str">
         <f t="shared" si="0"/>
@@ -6696,10 +6740,10 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="78" t="s">
+        <v>286</v>
+      </c>
+      <c r="B21" s="78" t="s">
         <v>287</v>
-      </c>
-      <c r="B21" s="78" t="s">
-        <v>288</v>
       </c>
       <c r="H21" t="str">
         <f t="shared" si="0"/>
@@ -6708,10 +6752,10 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="78" t="s">
+        <v>288</v>
+      </c>
+      <c r="B22" s="78" t="s">
         <v>289</v>
-      </c>
-      <c r="B22" s="78" t="s">
-        <v>290</v>
       </c>
       <c r="H22" t="str">
         <f t="shared" si="0"/>
@@ -6720,10 +6764,10 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="78" t="s">
+        <v>290</v>
+      </c>
+      <c r="B23" s="78" t="s">
         <v>291</v>
-      </c>
-      <c r="B23" s="78" t="s">
-        <v>292</v>
       </c>
       <c r="H23" t="str">
         <f t="shared" si="0"/>
@@ -6732,10 +6776,10 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="78" t="s">
+        <v>292</v>
+      </c>
+      <c r="B24" s="78" t="s">
         <v>293</v>
-      </c>
-      <c r="B24" s="78" t="s">
-        <v>294</v>
       </c>
       <c r="H24" t="str">
         <f t="shared" si="0"/>
@@ -6744,10 +6788,10 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="78" t="s">
+        <v>294</v>
+      </c>
+      <c r="B25" s="78" t="s">
         <v>295</v>
-      </c>
-      <c r="B25" s="78" t="s">
-        <v>296</v>
       </c>
       <c r="H25" t="str">
         <f t="shared" si="0"/>
@@ -6756,10 +6800,10 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="78" t="s">
+        <v>296</v>
+      </c>
+      <c r="B26" s="78" t="s">
         <v>297</v>
-      </c>
-      <c r="B26" s="78" t="s">
-        <v>298</v>
       </c>
       <c r="H26" t="str">
         <f t="shared" si="0"/>
@@ -6768,10 +6812,10 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="78" t="s">
+        <v>298</v>
+      </c>
+      <c r="B27" s="78" t="s">
         <v>299</v>
-      </c>
-      <c r="B27" s="78" t="s">
-        <v>300</v>
       </c>
       <c r="H27" t="str">
         <f t="shared" si="0"/>
@@ -6780,10 +6824,10 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="78" t="s">
+        <v>300</v>
+      </c>
+      <c r="B28" s="78" t="s">
         <v>301</v>
-      </c>
-      <c r="B28" s="78" t="s">
-        <v>302</v>
       </c>
       <c r="H28" t="str">
         <f t="shared" si="0"/>
@@ -6792,10 +6836,10 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="78" t="s">
+        <v>302</v>
+      </c>
+      <c r="B29" s="78" t="s">
         <v>303</v>
-      </c>
-      <c r="B29" s="78" t="s">
-        <v>304</v>
       </c>
       <c r="H29" t="str">
         <f t="shared" si="0"/>
@@ -6804,10 +6848,10 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="78" t="s">
+        <v>304</v>
+      </c>
+      <c r="B30" s="78" t="s">
         <v>305</v>
-      </c>
-      <c r="B30" s="78" t="s">
-        <v>306</v>
       </c>
       <c r="H30" t="str">
         <f t="shared" si="0"/>
@@ -6816,10 +6860,10 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="78" t="s">
+        <v>306</v>
+      </c>
+      <c r="B31" s="78" t="s">
         <v>307</v>
-      </c>
-      <c r="B31" s="78" t="s">
-        <v>308</v>
       </c>
       <c r="H31" t="str">
         <f t="shared" si="0"/>
@@ -6828,10 +6872,10 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="78" t="s">
+        <v>308</v>
+      </c>
+      <c r="B32" s="78" t="s">
         <v>309</v>
-      </c>
-      <c r="B32" s="78" t="s">
-        <v>310</v>
       </c>
       <c r="H32" t="str">
         <f t="shared" si="0"/>
@@ -6840,10 +6884,10 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="78" t="s">
+        <v>310</v>
+      </c>
+      <c r="B33" s="78" t="s">
         <v>311</v>
-      </c>
-      <c r="B33" s="78" t="s">
-        <v>312</v>
       </c>
       <c r="H33" t="str">
         <f t="shared" si="0"/>
@@ -6852,10 +6896,10 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="78" t="s">
+        <v>312</v>
+      </c>
+      <c r="B34" s="78" t="s">
         <v>313</v>
-      </c>
-      <c r="B34" s="78" t="s">
-        <v>314</v>
       </c>
       <c r="H34" t="str">
         <f t="shared" si="0"/>
@@ -6864,10 +6908,10 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="78" t="s">
+        <v>314</v>
+      </c>
+      <c r="B35" s="78" t="s">
         <v>315</v>
-      </c>
-      <c r="B35" s="78" t="s">
-        <v>316</v>
       </c>
       <c r="H35" t="str">
         <f t="shared" si="0"/>
@@ -6876,10 +6920,10 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="78" t="s">
+        <v>316</v>
+      </c>
+      <c r="B36" s="78" t="s">
         <v>317</v>
-      </c>
-      <c r="B36" s="78" t="s">
-        <v>318</v>
       </c>
       <c r="H36" t="str">
         <f t="shared" si="0"/>
@@ -6888,10 +6932,10 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="78" t="s">
+        <v>318</v>
+      </c>
+      <c r="B37" s="78" t="s">
         <v>319</v>
-      </c>
-      <c r="B37" s="78" t="s">
-        <v>320</v>
       </c>
       <c r="H37" t="str">
         <f t="shared" si="0"/>
@@ -6900,10 +6944,10 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="78" t="s">
+        <v>320</v>
+      </c>
+      <c r="B38" s="78" t="s">
         <v>321</v>
-      </c>
-      <c r="B38" s="78" t="s">
-        <v>322</v>
       </c>
       <c r="H38" t="str">
         <f t="shared" si="0"/>
@@ -6912,10 +6956,10 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="78" t="s">
+        <v>322</v>
+      </c>
+      <c r="B39" s="78" t="s">
         <v>323</v>
-      </c>
-      <c r="B39" s="78" t="s">
-        <v>324</v>
       </c>
       <c r="H39" t="str">
         <f t="shared" si="0"/>
@@ -6942,106 +6986,106 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.3">
       <c r="A1" s="79" t="s">
+        <v>324</v>
+      </c>
+      <c r="B1" s="77" t="s">
         <v>325</v>
-      </c>
-      <c r="B1" s="77" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="78" t="s">
+        <v>326</v>
+      </c>
+      <c r="B2" s="78" t="s">
         <v>327</v>
-      </c>
-      <c r="B2" s="78" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="78" t="s">
+        <v>328</v>
+      </c>
+      <c r="B3" s="78" t="s">
         <v>329</v>
-      </c>
-      <c r="B3" s="78" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="78" t="s">
+        <v>330</v>
+      </c>
+      <c r="B4" s="78" t="s">
         <v>331</v>
-      </c>
-      <c r="B4" s="78" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="78" t="s">
+        <v>332</v>
+      </c>
+      <c r="B5" s="78" t="s">
         <v>333</v>
-      </c>
-      <c r="B5" s="78" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="78" t="s">
+        <v>334</v>
+      </c>
+      <c r="B6" s="78" t="s">
         <v>335</v>
-      </c>
-      <c r="B6" s="78" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="78" t="s">
+        <v>336</v>
+      </c>
+      <c r="B7" s="78" t="s">
         <v>337</v>
-      </c>
-      <c r="B7" s="78" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="78" t="s">
+        <v>338</v>
+      </c>
+      <c r="B8" s="78" t="s">
         <v>339</v>
-      </c>
-      <c r="B8" s="78" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="78" t="s">
+        <v>340</v>
+      </c>
+      <c r="B9" s="78" t="s">
         <v>341</v>
-      </c>
-      <c r="B9" s="78" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="78" t="s">
+        <v>342</v>
+      </c>
+      <c r="B10" s="78" t="s">
         <v>343</v>
-      </c>
-      <c r="B10" s="78" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="78" t="s">
+        <v>344</v>
+      </c>
+      <c r="B11" s="78" t="s">
         <v>345</v>
-      </c>
-      <c r="B11" s="78" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="78" t="s">
+        <v>346</v>
+      </c>
+      <c r="B12" s="78" t="s">
         <v>347</v>
-      </c>
-      <c r="B12" s="78" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="78" t="s">
+        <v>348</v>
+      </c>
+      <c r="B13" s="78" t="s">
         <v>349</v>
-      </c>
-      <c r="B13" s="78" t="s">
-        <v>350</v>
       </c>
     </row>
   </sheetData>

</xml_diff>